<commit_message>
re-saved a few spreadsheets.
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/2014 Wenatchee Modeling Data - Final.xlsx
+++ b/analysis/data/raw_data/2014 Wenatchee Modeling Data - Final.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/kevin_see_dfw_wa_gov/Documents/Documents/Git/MyProjects/UCSthdReddObsErr/analysis/data/raw_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_3211ECB0090A2EB37B4BAC7651F835ADEA0EB938" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E242CB1C-FFA0-4279-82A4-D23E2F3792EF}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="22960" windowHeight="14440"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey data" sheetId="1" r:id="rId1"/>
@@ -14,8 +20,17 @@
     <sheet name="reach associations" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,13 +39,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Murdoch, Andrew R (DFW)</author>
     <author xml:space="preserve">Frady, Charles H </author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -54,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -78,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -102,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="1">
+    <comment ref="L1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -131,12 +146,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author xml:space="preserve">Frady, Charles H </author>
   </authors>
   <commentList>
-    <comment ref="G20" authorId="0">
+    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -160,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G21" authorId="0">
+    <comment ref="G21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -184,7 +199,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0">
+    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1044,7 +1059,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1220,6 +1235,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1241,7 +1259,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1285,7 +1309,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1603,7 +1633,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1611,23 +1641,23 @@
       <selection pane="bottomLeft" activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="8.81640625" style="2"/>
     <col min="3" max="3" width="10" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="7.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="2"/>
-    <col min="7" max="7" width="10.83203125" style="23" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="33" customWidth="1"/>
-    <col min="9" max="11" width="12.5" style="21" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="10.5" style="4" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="38" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="7.81640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" style="2"/>
+    <col min="7" max="7" width="10.81640625" style="23" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" style="33" customWidth="1"/>
+    <col min="9" max="11" width="12.453125" style="21" customWidth="1"/>
+    <col min="12" max="12" width="11.1796875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="10.453125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="19.36328125" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="46.5" customHeight="1">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1671,7 +1701,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
@@ -1716,7 +1746,7 @@
         <v>5.0852257064734939E-6</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
@@ -1761,7 +1791,7 @@
         <v>7.6278385597102404E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -1806,7 +1836,7 @@
         <v>7.6278385597102404E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -1851,7 +1881,7 @@
         <v>7.6278385597102404E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -1896,7 +1926,7 @@
         <v>1.5255677119420481E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -1941,7 +1971,7 @@
         <v>2.2883515679130722E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
@@ -1986,7 +2016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -2031,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
@@ -2076,7 +2106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -2121,7 +2151,7 @@
         <v>4.7102437895017346E-6</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
@@ -2166,7 +2196,7 @@
         <v>9.4204875790034692E-6</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -2211,7 +2241,7 @@
         <v>1.4130731368505204E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
@@ -2256,7 +2286,7 @@
         <v>2.8261462737010408E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
@@ -2301,7 +2331,7 @@
         <v>2.8261462737010408E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
@@ -2346,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -2391,7 +2421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
@@ -2436,7 +2466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
@@ -2481,7 +2511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
@@ -2526,7 +2556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -2571,7 +2601,7 @@
         <v>2.4224583400228463E-6</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
@@ -2616,7 +2646,7 @@
         <v>4.8449166800456927E-6</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
@@ -2661,7 +2691,7 @@
         <v>7.267375020068539E-6</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
@@ -2706,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>33</v>
       </c>
@@ -2751,7 +2781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
@@ -2796,7 +2826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>33</v>
       </c>
@@ -2841,7 +2871,7 @@
         <v>7.2170420160557098E-6</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
@@ -2886,7 +2916,7 @@
         <v>7.2170420160557098E-6</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -2931,7 +2961,7 @@
         <v>4.3302252096334259E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
@@ -2976,7 +3006,7 @@
         <v>7.9387462176612808E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>33</v>
       </c>
@@ -3021,7 +3051,7 @@
         <v>2.1651126048167129E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>33</v>
       </c>
@@ -3066,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -3111,7 +3141,7 @@
         <v>4.9505254231228315E-6</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -3156,7 +3186,7 @@
         <v>7.4257881346842481E-6</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
@@ -3201,7 +3231,7 @@
         <v>9.901050846245663E-6</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>32</v>
       </c>
@@ -3246,7 +3276,7 @@
         <v>1.7326838980929912E-5</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
@@ -3291,7 +3321,7 @@
         <v>2.2277364404052743E-5</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>32</v>
       </c>
@@ -3336,7 +3366,7 @@
         <v>2.9703152538736992E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>32</v>
       </c>
@@ -3381,7 +3411,7 @@
         <v>3.7128940673421238E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>32</v>
       </c>
@@ -3426,7 +3456,7 @@
         <v>2.9703152538736992E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>32</v>
       </c>
@@ -3471,7 +3501,7 @@
         <v>7.4257881346842481E-6</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>32</v>
       </c>
@@ -3516,7 +3546,7 @@
         <v>7.4257881346842481E-6</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>32</v>
       </c>
@@ -3561,7 +3591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>32</v>
       </c>
@@ -3606,7 +3636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>32</v>
       </c>
@@ -3651,7 +3681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>32</v>
       </c>
@@ -3696,7 +3726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>32</v>
       </c>
@@ -3741,7 +3771,7 @@
         <v>4.7340749141963774E-6</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>32</v>
       </c>
@@ -3786,7 +3816,7 @@
         <v>4.7340749141963774E-6</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>32</v>
       </c>
@@ -3831,7 +3861,7 @@
         <v>1.5780249713987925E-6</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>32</v>
       </c>
@@ -3876,7 +3906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>32</v>
       </c>
@@ -3921,7 +3951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>32</v>
       </c>
@@ -3966,7 +3996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>32</v>
       </c>
@@ -4011,7 +4041,7 @@
         <v>8.2647275560525671E-6</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>32</v>
       </c>
@@ -4056,7 +4086,7 @@
         <v>2.0661818890131419E-5</v>
       </c>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>32</v>
       </c>
@@ -4101,7 +4131,7 @@
         <v>3.7191274002236553E-5</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>32</v>
       </c>
@@ -4146,7 +4176,7 @@
         <v>5.7853092892367975E-5</v>
       </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>32</v>
       </c>
@@ -4191,7 +4221,7 @@
         <v>8.2647275560525675E-5</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>32</v>
       </c>
@@ -4236,7 +4266,7 @@
         <v>8.2647275560525675E-5</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>32</v>
       </c>
@@ -4281,7 +4311,7 @@
         <v>8.6779639338551966E-5</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>32</v>
       </c>
@@ -4326,7 +4356,7 @@
         <v>7.8514911782499397E-5</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>32</v>
       </c>
@@ -4371,7 +4401,7 @@
         <v>1.2397091334078852E-5</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>32</v>
       </c>
@@ -4416,7 +4446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>32</v>
       </c>
@@ -4461,7 +4491,7 @@
         <v>8.9320795223427532E-5</v>
       </c>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>32</v>
       </c>
@@ -4506,7 +4536,7 @@
         <v>8.9320795223427532E-5</v>
       </c>
     </row>
-    <row r="65" spans="1:14">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>32</v>
       </c>
@@ -4551,7 +4581,7 @@
         <v>1.3398119283514128E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:14">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>32</v>
       </c>
@@ -4596,7 +4626,7 @@
         <v>1.3398119283514128E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>32</v>
       </c>
@@ -4641,7 +4671,7 @@
         <v>1.3398119283514128E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>32</v>
       </c>
@@ -4686,7 +4716,7 @@
         <v>1.7864159044685506E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>32</v>
       </c>
@@ -4731,7 +4761,7 @@
         <v>1.7864159044685506E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>32</v>
       </c>
@@ -4776,7 +4806,7 @@
         <v>2.0428809196723196E-6</v>
       </c>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>32</v>
       </c>
@@ -4821,7 +4851,7 @@
         <v>8.1715236786892783E-6</v>
       </c>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>32</v>
       </c>
@@ -4866,7 +4896,7 @@
         <v>1.4300166437706238E-5</v>
       </c>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>32</v>
       </c>
@@ -4911,7 +4941,7 @@
         <v>2.1450249656559358E-5</v>
       </c>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>32</v>
       </c>
@@ -4956,7 +4986,7 @@
         <v>2.8600332875412477E-5</v>
       </c>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>32</v>
       </c>
@@ -5001,7 +5031,7 @@
         <v>2.9621773335248635E-5</v>
       </c>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>32</v>
       </c>
@@ -5046,7 +5076,7 @@
         <v>2.1450249656559358E-5</v>
       </c>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>32</v>
       </c>
@@ -5091,7 +5121,7 @@
         <v>1.9407368736887038E-5</v>
       </c>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>32</v>
       </c>
@@ -5136,7 +5166,7 @@
         <v>9.1929641385254383E-6</v>
       </c>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>32</v>
       </c>
@@ -5181,7 +5211,7 @@
         <v>9.1929641385254383E-6</v>
       </c>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>33</v>
       </c>
@@ -5226,7 +5256,7 @@
         <v>1.5739209952661241E-6</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>33</v>
       </c>
@@ -5271,7 +5301,7 @@
         <v>1.2264015030467061E-6</v>
       </c>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>33</v>
       </c>
@@ -5316,7 +5346,7 @@
         <v>4.2634643104076908E-6</v>
       </c>
     </row>
-    <row r="83" spans="1:14">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
         <v>33</v>
       </c>
@@ -5361,7 +5391,7 @@
         <v>5.6040563667051953E-6</v>
       </c>
     </row>
-    <row r="84" spans="1:14">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>32</v>
       </c>
@@ -5406,7 +5436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>32</v>
       </c>
@@ -5451,7 +5481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>32</v>
       </c>
@@ -5496,7 +5526,7 @@
         <v>2.5081128797604869E-6</v>
       </c>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>32</v>
       </c>
@@ -5541,7 +5571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>32</v>
       </c>
@@ -5586,7 +5616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:14">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>32</v>
       </c>
@@ -5631,7 +5661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:14">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A90" s="21" t="s">
         <v>32</v>
       </c>
@@ -5677,7 +5707,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L90">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L90">
     <sortCondition descending="1" ref="C2:C90"/>
     <sortCondition ref="B2:B90"/>
     <sortCondition ref="E2:E90"/>
@@ -5694,7 +5724,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L144"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -5702,19 +5732,19 @@
       <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="2"/>
-    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="2"/>
-    <col min="4" max="4" width="12.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="8.81640625" style="2"/>
+    <col min="2" max="2" width="15.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" style="2"/>
+    <col min="4" max="4" width="12.36328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="28">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
@@ -5740,7 +5770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>2014</v>
       </c>
@@ -5764,7 +5794,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2014</v>
       </c>
@@ -5788,7 +5818,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2014</v>
       </c>
@@ -5812,7 +5842,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>2014</v>
       </c>
@@ -5839,7 +5869,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>2014</v>
       </c>
@@ -5866,7 +5896,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="15" customFormat="1">
+    <row r="7" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25">
         <v>2014</v>
       </c>
@@ -5893,7 +5923,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>2014</v>
       </c>
@@ -5920,7 +5950,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>2014</v>
       </c>
@@ -5947,7 +5977,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>2014</v>
       </c>
@@ -5974,7 +6004,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>2014</v>
       </c>
@@ -6001,7 +6031,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>2014</v>
       </c>
@@ -6028,7 +6058,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>2014</v>
       </c>
@@ -6055,7 +6085,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>2014</v>
       </c>
@@ -6079,7 +6109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>2014</v>
       </c>
@@ -6103,7 +6133,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>2014</v>
       </c>
@@ -6127,7 +6157,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>2014</v>
       </c>
@@ -6151,7 +6181,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>2014</v>
       </c>
@@ -6178,7 +6208,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>2014</v>
       </c>
@@ -6205,7 +6235,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>2014</v>
       </c>
@@ -6229,7 +6259,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>2014</v>
       </c>
@@ -6256,7 +6286,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>2014</v>
       </c>
@@ -6283,7 +6313,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>2014</v>
       </c>
@@ -6307,7 +6337,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>2014</v>
       </c>
@@ -6331,7 +6361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>2014</v>
       </c>
@@ -6355,7 +6385,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>2014</v>
       </c>
@@ -6382,7 +6412,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>2014</v>
       </c>
@@ -6409,7 +6439,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>2014</v>
       </c>
@@ -6439,7 +6469,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>2014</v>
       </c>
@@ -6469,7 +6499,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>2014</v>
       </c>
@@ -6502,7 +6532,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="13">
         <v>2014</v>
       </c>
@@ -6540,7 +6570,7 @@
         <v>11.333301502374448</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>2014</v>
       </c>
@@ -6578,7 +6608,7 @@
         <v>12.386820953470398</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>2014</v>
       </c>
@@ -6605,87 +6635,87 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>2014</v>
       </c>
@@ -6711,7 +6741,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>2014</v>
       </c>
@@ -6737,7 +6767,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>2014</v>
       </c>
@@ -6763,7 +6793,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>2014</v>
       </c>
@@ -6786,7 +6816,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>2014</v>
       </c>
@@ -6812,7 +6842,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>2014</v>
       </c>
@@ -6835,7 +6865,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>2014</v>
       </c>
@@ -6858,7 +6888,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>2014</v>
       </c>
@@ -6881,7 +6911,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>2014</v>
       </c>
@@ -6904,7 +6934,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>2014</v>
       </c>
@@ -6930,7 +6960,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>2014</v>
       </c>
@@ -6953,7 +6983,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>2014</v>
       </c>
@@ -6979,7 +7009,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>2014</v>
       </c>
@@ -7005,7 +7035,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>2014</v>
       </c>
@@ -7028,7 +7058,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>2014</v>
       </c>
@@ -7054,7 +7084,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>2014</v>
       </c>
@@ -7080,7 +7110,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>2014</v>
       </c>
@@ -7106,7 +7136,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>2014</v>
       </c>
@@ -7132,7 +7162,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>2014</v>
       </c>
@@ -7155,7 +7185,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>2014</v>
       </c>
@@ -7181,7 +7211,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>2014</v>
       </c>
@@ -7207,7 +7237,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>2014</v>
       </c>
@@ -7233,7 +7263,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>2014</v>
       </c>
@@ -7259,7 +7289,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>2014</v>
       </c>
@@ -7282,7 +7312,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>2014</v>
       </c>
@@ -7308,7 +7338,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>2014</v>
       </c>
@@ -7337,7 +7367,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>2014</v>
       </c>
@@ -7360,7 +7390,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>2014</v>
       </c>
@@ -7386,7 +7416,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>2014</v>
       </c>
@@ -7417,7 +7447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>2014</v>
       </c>
@@ -7448,7 +7478,7 @@
         <v>11.970833964301139</v>
       </c>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>2014</v>
       </c>
@@ -7479,7 +7509,7 @@
         <v>11.626079058982626</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>2014</v>
       </c>
@@ -7499,7 +7529,7 @@
         <v>41759</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>2014</v>
       </c>
@@ -7516,7 +7546,7 @@
         <v>41759</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>2014</v>
       </c>
@@ -7542,7 +7572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>2014</v>
       </c>
@@ -7568,7 +7598,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>2014</v>
       </c>
@@ -7594,7 +7624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>2014</v>
       </c>
@@ -7620,7 +7650,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>2014</v>
       </c>
@@ -7646,7 +7676,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>2014</v>
       </c>
@@ -7672,7 +7702,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>2014</v>
       </c>
@@ -7695,7 +7725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>2014</v>
       </c>
@@ -7721,7 +7751,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>2014</v>
       </c>
@@ -7747,7 +7777,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>2014</v>
       </c>
@@ -7773,7 +7803,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>2014</v>
       </c>
@@ -7799,7 +7829,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>2014</v>
       </c>
@@ -7825,7 +7855,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>2014</v>
       </c>
@@ -7851,7 +7881,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>2014</v>
       </c>
@@ -7877,7 +7907,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>2014</v>
       </c>
@@ -7903,7 +7933,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>2014</v>
       </c>
@@ -7929,7 +7959,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>2014</v>
       </c>
@@ -7955,7 +7985,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>2014</v>
       </c>
@@ -7981,7 +8011,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>2014</v>
       </c>
@@ -8007,7 +8037,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
         <v>2014</v>
       </c>
@@ -8033,7 +8063,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
         <v>2014</v>
       </c>
@@ -8059,7 +8089,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="2">
         <v>2014</v>
       </c>
@@ -8085,7 +8115,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="2">
         <v>2014</v>
       </c>
@@ -8111,7 +8141,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="2">
         <v>2014</v>
       </c>
@@ -8137,7 +8167,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="2">
         <v>2014</v>
       </c>
@@ -8163,7 +8193,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" s="2">
         <v>2014</v>
       </c>
@@ -8189,7 +8219,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="2">
         <v>2014</v>
       </c>
@@ -8215,7 +8245,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" s="2">
         <v>2014</v>
       </c>
@@ -8241,7 +8271,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" s="2">
         <v>2014</v>
       </c>
@@ -8267,7 +8297,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="2">
         <v>2014</v>
       </c>
@@ -8293,7 +8323,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="2">
         <v>2014</v>
       </c>
@@ -8319,7 +8349,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="2">
         <v>2014</v>
       </c>
@@ -8345,7 +8375,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" s="2">
         <v>2014</v>
       </c>
@@ -8371,7 +8401,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="2">
         <v>2014</v>
       </c>
@@ -8397,7 +8427,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="2">
         <v>2014</v>
       </c>
@@ -8423,7 +8453,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="2">
         <v>2014</v>
       </c>
@@ -8449,7 +8479,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="2">
         <v>2014</v>
       </c>
@@ -8475,7 +8505,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="2">
         <v>2014</v>
       </c>
@@ -8495,7 +8525,7 @@
         <v>41788</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" s="2">
         <v>2014</v>
       </c>
@@ -8515,7 +8545,7 @@
         <v>41788</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" s="2">
         <v>2014</v>
       </c>
@@ -8535,7 +8565,7 @@
         <v>41788</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="2">
         <v>2014</v>
       </c>
@@ -8555,7 +8585,7 @@
         <v>41788</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="2">
         <v>2014</v>
       </c>
@@ -8572,7 +8602,7 @@
         <v>41788</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="2">
         <v>2014</v>
       </c>
@@ -8592,7 +8622,7 @@
         <v>41788</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="2">
         <v>2014</v>
       </c>
@@ -8612,7 +8642,7 @@
         <v>41787</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" s="2">
         <v>2014</v>
       </c>
@@ -8632,7 +8662,7 @@
         <v>41792</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="2">
         <v>2014</v>
       </c>
@@ -8652,7 +8682,7 @@
         <v>41792</v>
       </c>
     </row>
-    <row r="129" spans="2:8">
+    <row r="129" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B129" s="2" t="s">
         <v>32</v>
       </c>
@@ -8672,7 +8702,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="130" spans="2:8">
+    <row r="130" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B130" s="2" t="s">
         <v>32</v>
       </c>
@@ -8692,7 +8722,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="131" spans="2:8">
+    <row r="131" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B131" s="2" t="s">
         <v>32</v>
       </c>
@@ -8715,7 +8745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="132" spans="2:8">
+    <row r="132" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B132" s="2" t="s">
         <v>32</v>
       </c>
@@ -8735,7 +8765,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="2:8">
+    <row r="133" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B133" s="2" t="s">
         <v>32</v>
       </c>
@@ -8758,7 +8788,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="134" spans="2:8">
+    <row r="134" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B134" s="2" t="s">
         <v>32</v>
       </c>
@@ -8781,7 +8811,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="135" spans="2:8">
+    <row r="135" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B135" s="2" t="s">
         <v>32</v>
       </c>
@@ -8804,7 +8834,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="136" spans="2:8">
+    <row r="136" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B136" s="2" t="s">
         <v>32</v>
       </c>
@@ -8827,7 +8857,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="137" spans="2:8">
+    <row r="137" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B137" s="2" t="s">
         <v>32</v>
       </c>
@@ -8850,7 +8880,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="138" spans="2:8">
+    <row r="138" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B138" s="2" t="s">
         <v>32</v>
       </c>
@@ -8873,7 +8903,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="139" spans="2:8">
+    <row r="139" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B139" s="2" t="s">
         <v>32</v>
       </c>
@@ -8896,7 +8926,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="140" spans="2:8">
+    <row r="140" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B140" s="2" t="s">
         <v>32</v>
       </c>
@@ -8919,7 +8949,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="141" spans="2:8">
+    <row r="141" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B141" s="2" t="s">
         <v>32</v>
       </c>
@@ -8942,7 +8972,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="142" spans="2:8">
+    <row r="142" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B142" s="2" t="s">
         <v>32</v>
       </c>
@@ -8959,7 +8989,7 @@
         <v>41787</v>
       </c>
     </row>
-    <row r="143" spans="2:8">
+    <row r="143" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B143" s="2" t="s">
         <v>32</v>
       </c>
@@ -8976,7 +9006,7 @@
         <v>41787</v>
       </c>
     </row>
-    <row r="144" spans="2:8">
+    <row r="144" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B144" s="2" t="s">
         <v>32</v>
       </c>
@@ -8994,7 +9024,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H128">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H128">
     <sortCondition ref="C2:C128"/>
     <sortCondition ref="H2:H128"/>
   </sortState>
@@ -9011,26 +9041,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.36328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
@@ -9041,7 +9071,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -9052,7 +9082,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>48</v>
       </c>
@@ -9063,7 +9093,7 @@
         <v>27.9</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>58</v>
       </c>
@@ -9074,7 +9104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
@@ -9085,7 +9115,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>50</v>
       </c>
@@ -9096,7 +9126,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
@@ -9107,7 +9137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="27" t="s">
         <v>197</v>
       </c>
@@ -9122,7 +9152,7 @@
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>198</v>
       </c>
@@ -9141,7 +9171,7 @@
         <v>24.450000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
         <v>199</v>
       </c>
@@ -9160,7 +9190,7 @@
         <v>33.450000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
         <v>201</v>
       </c>
@@ -9179,7 +9209,7 @@
         <v>35.65</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
         <v>202</v>
       </c>
@@ -9198,7 +9228,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
         <v>203</v>
       </c>
@@ -9217,7 +9247,7 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="25" t="s">
         <v>204</v>
       </c>
@@ -9236,7 +9266,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="25" t="s">
         <v>206</v>
       </c>
@@ -9255,7 +9285,7 @@
         <v>29.35</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="25" t="s">
         <v>207</v>
       </c>
@@ -9274,7 +9304,7 @@
         <v>26.650000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="25" t="s">
         <v>208</v>
       </c>
@@ -9293,7 +9323,7 @@
         <v>36.450000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="25" t="s">
         <v>97</v>
       </c>
@@ -9319,24 +9349,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="41.6640625" style="24" customWidth="1"/>
-    <col min="7" max="7" width="12.5" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="28" customWidth="1"/>
-    <col min="9" max="12" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.36328125" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="24" customWidth="1"/>
+    <col min="4" max="4" width="41.6328125" style="24" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" style="28" customWidth="1"/>
+    <col min="9" max="12" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -9374,7 +9404,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="24" customFormat="1">
+    <row r="2" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
         <v>32</v>
       </c>
@@ -9404,7 +9434,7 @@
       <c r="K2" s="34"/>
       <c r="L2" s="34"/>
     </row>
-    <row r="3" spans="1:12" s="24" customFormat="1">
+    <row r="3" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
         <v>32</v>
       </c>
@@ -9434,7 +9464,7 @@
       <c r="K3" s="34"/>
       <c r="L3" s="34"/>
     </row>
-    <row r="4" spans="1:12" s="24" customFormat="1">
+    <row r="4" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="28" t="s">
         <v>32</v>
       </c>
@@ -9464,7 +9494,7 @@
       <c r="K4" s="34"/>
       <c r="L4" s="34"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="28" t="s">
         <v>32</v>
       </c>
@@ -9494,7 +9524,7 @@
       <c r="K5" s="28"/>
       <c r="L5" s="28"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="28" t="s">
         <v>32</v>
       </c>
@@ -9524,7 +9554,7 @@
       <c r="K6" s="28"/>
       <c r="L6" s="28"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="28" t="s">
         <v>32</v>
       </c>
@@ -9554,7 +9584,7 @@
       <c r="K7" s="28"/>
       <c r="L7" s="28"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="28" t="s">
         <v>32</v>
       </c>
@@ -9584,7 +9614,7 @@
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
     </row>
-    <row r="9" spans="1:12" s="24" customFormat="1">
+    <row r="9" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="28" t="s">
         <v>32</v>
       </c>
@@ -9614,7 +9644,7 @@
       <c r="K9" s="28"/>
       <c r="L9" s="28"/>
     </row>
-    <row r="10" spans="1:12" s="24" customFormat="1">
+    <row r="10" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="28" t="s">
         <v>32</v>
       </c>
@@ -9644,7 +9674,7 @@
       <c r="K10" s="28"/>
       <c r="L10" s="28"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
         <v>32</v>
       </c>
@@ -9674,7 +9704,7 @@
       <c r="K11" s="28"/>
       <c r="L11" s="28"/>
     </row>
-    <row r="12" spans="1:12" s="24" customFormat="1">
+    <row r="12" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="28" t="s">
         <v>32</v>
       </c>
@@ -9704,7 +9734,7 @@
       <c r="K12" s="28"/>
       <c r="L12" s="28"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="28" t="s">
         <v>32</v>
       </c>
@@ -9734,7 +9764,7 @@
       <c r="K13" s="28"/>
       <c r="L13" s="28"/>
     </row>
-    <row r="14" spans="1:12" s="24" customFormat="1">
+    <row r="14" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
         <v>32</v>
       </c>
@@ -9764,7 +9794,7 @@
       <c r="K14" s="28"/>
       <c r="L14" s="28"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="28" t="s">
         <v>32</v>
       </c>
@@ -9794,7 +9824,7 @@
       <c r="K15" s="28"/>
       <c r="L15" s="28"/>
     </row>
-    <row r="16" spans="1:12" s="24" customFormat="1">
+    <row r="16" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
         <v>32</v>
       </c>
@@ -9824,7 +9854,7 @@
       <c r="K16" s="28"/>
       <c r="L16" s="28"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
         <v>33</v>
       </c>
@@ -9862,7 +9892,7 @@
         <v>-120.18810000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="28" t="s">
         <v>33</v>
       </c>
@@ -9900,7 +9930,7 @@
         <v>-120.1066</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
         <v>33</v>
       </c>
@@ -9938,7 +9968,7 @@
         <v>-120.0664</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
         <v>33</v>
       </c>
@@ -9976,7 +10006,7 @@
         <v>-120.1173</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="28" t="s">
         <v>33</v>
       </c>
@@ -10014,7 +10044,7 @@
         <v>-120.12520000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="28" t="s">
         <v>33</v>
       </c>
@@ -10052,7 +10082,7 @@
         <v>-120.01609999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="28" t="s">
         <v>33</v>
       </c>
@@ -10090,7 +10120,7 @@
         <v>-120.0209</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>33</v>
       </c>
@@ -10129,7 +10159,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A19:K26">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A19:K26">
     <sortCondition descending="1" ref="B19:B26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10142,21 +10172,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L5239"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B16:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>209</v>
       </c>
@@ -10164,7 +10194,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -10172,7 +10202,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -10180,7 +10210,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -10188,7 +10218,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -10196,7 +10226,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -10204,7 +10234,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="24" t="s">
         <v>34</v>
       </c>
@@ -10212,7 +10242,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="24" t="s">
         <v>39</v>
       </c>
@@ -10220,7 +10250,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="24" t="s">
         <v>42</v>
       </c>
@@ -10228,7 +10258,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="24" t="s">
         <v>45</v>
       </c>
@@ -10236,94 +10266,94 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" s="15"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="24"/>
       <c r="B13" s="24"/>
     </row>
-    <row r="3013" spans="6:12">
+    <row r="3013" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F3013" s="9"/>
       <c r="L3013" s="9"/>
     </row>
-    <row r="3014" spans="6:12">
+    <row r="3014" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F3014" s="9"/>
       <c r="L3014" s="9"/>
     </row>
-    <row r="3015" spans="6:12">
+    <row r="3015" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F3015" s="9"/>
       <c r="L3015" s="9"/>
     </row>
-    <row r="3016" spans="6:12">
+    <row r="3016" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F3016" s="9"/>
       <c r="L3016" s="9"/>
     </row>
-    <row r="3017" spans="6:12">
+    <row r="3017" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F3017" s="9"/>
       <c r="L3017" s="9"/>
     </row>
-    <row r="3688" spans="6:12">
+    <row r="3688" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F3688" s="9"/>
       <c r="L3688" s="9"/>
     </row>
-    <row r="3689" spans="6:12">
+    <row r="3689" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F3689" s="9"/>
       <c r="L3689" s="9"/>
     </row>
-    <row r="3690" spans="6:12">
+    <row r="3690" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F3690" s="9"/>
       <c r="L3690" s="9"/>
     </row>
-    <row r="3691" spans="6:12">
+    <row r="3691" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F3691" s="9"/>
       <c r="L3691" s="9"/>
     </row>
-    <row r="3692" spans="6:12">
+    <row r="3692" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F3692" s="9"/>
       <c r="L3692" s="9"/>
     </row>
-    <row r="3693" spans="6:12">
+    <row r="3693" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F3693" s="9"/>
       <c r="L3693" s="9"/>
     </row>
-    <row r="4356" spans="6:12">
+    <row r="4356" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F4356" s="9"/>
       <c r="L4356" s="9"/>
     </row>
-    <row r="4357" spans="6:12">
+    <row r="4357" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F4357" s="9"/>
       <c r="L4357" s="9"/>
     </row>
-    <row r="4358" spans="6:12">
+    <row r="4358" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F4358" s="9"/>
       <c r="L4358" s="9"/>
     </row>
-    <row r="4359" spans="6:12">
+    <row r="4359" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F4359" s="9"/>
       <c r="L4359" s="9"/>
     </row>
-    <row r="4360" spans="6:12">
+    <row r="4360" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F4360" s="9"/>
       <c r="L4360" s="9"/>
     </row>
-    <row r="4361" spans="6:12">
+    <row r="4361" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F4361" s="9"/>
       <c r="L4361" s="9"/>
     </row>
-    <row r="5236" spans="6:12">
+    <row r="5236" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F5236" s="9"/>
       <c r="L5236" s="9"/>
     </row>
-    <row r="5237" spans="6:12">
+    <row r="5237" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F5237" s="9"/>
       <c r="L5237" s="9"/>
     </row>
-    <row r="5238" spans="6:12">
+    <row r="5238" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F5238" s="9"/>
       <c r="L5238" s="9"/>
     </row>
-    <row r="5239" spans="6:12">
+    <row r="5239" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F5239" s="9"/>
       <c r="L5239" s="9"/>
     </row>
@@ -10338,133 +10368,133 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="D4166:D4282"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H5531" sqref="H5531"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4166" spans="4:4">
+    <row r="4166" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4166" s="9"/>
     </row>
-    <row r="4167" spans="4:4">
+    <row r="4167" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4167" s="9"/>
     </row>
-    <row r="4168" spans="4:4">
+    <row r="4168" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4168" s="9"/>
     </row>
-    <row r="4169" spans="4:4">
+    <row r="4169" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4169" s="9"/>
     </row>
-    <row r="4170" spans="4:4">
+    <row r="4170" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4170" s="9"/>
     </row>
-    <row r="4171" spans="4:4">
+    <row r="4171" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4171" s="9"/>
     </row>
-    <row r="4172" spans="4:4">
+    <row r="4172" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4172" s="9"/>
     </row>
-    <row r="4173" spans="4:4">
+    <row r="4173" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4173" s="9"/>
     </row>
-    <row r="4174" spans="4:4">
+    <row r="4174" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4174" s="9"/>
     </row>
-    <row r="4175" spans="4:4">
+    <row r="4175" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4175" s="9"/>
     </row>
-    <row r="4176" spans="4:4">
+    <row r="4176" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4176" s="9"/>
     </row>
-    <row r="4177" spans="4:4">
+    <row r="4177" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4177" s="9"/>
     </row>
-    <row r="4178" spans="4:4">
+    <row r="4178" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4178" s="9"/>
     </row>
-    <row r="4179" spans="4:4">
+    <row r="4179" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4179" s="9"/>
     </row>
-    <row r="4180" spans="4:4">
+    <row r="4180" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4180" s="9"/>
     </row>
-    <row r="4181" spans="4:4">
+    <row r="4181" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4181" s="9"/>
     </row>
-    <row r="4182" spans="4:4">
+    <row r="4182" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4182" s="9"/>
     </row>
-    <row r="4183" spans="4:4">
+    <row r="4183" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4183" s="9"/>
     </row>
-    <row r="4184" spans="4:4">
+    <row r="4184" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4184" s="9"/>
     </row>
-    <row r="4185" spans="4:4">
+    <row r="4185" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4185" s="9"/>
     </row>
-    <row r="4186" spans="4:4">
+    <row r="4186" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4186" s="9"/>
     </row>
-    <row r="4187" spans="4:4">
+    <row r="4187" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4187" s="9"/>
     </row>
-    <row r="4188" spans="4:4">
+    <row r="4188" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4188" s="9"/>
     </row>
-    <row r="4264" spans="4:4">
+    <row r="4264" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4264" s="9"/>
     </row>
-    <row r="4265" spans="4:4">
+    <row r="4265" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4265" s="9"/>
     </row>
-    <row r="4266" spans="4:4">
+    <row r="4266" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4266" s="9"/>
     </row>
-    <row r="4267" spans="4:4">
+    <row r="4267" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4267" s="9"/>
     </row>
-    <row r="4268" spans="4:4">
+    <row r="4268" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4268" s="9"/>
     </row>
-    <row r="4269" spans="4:4">
+    <row r="4269" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4269" s="9"/>
     </row>
-    <row r="4273" spans="4:4">
+    <row r="4273" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4273" s="9"/>
     </row>
-    <row r="4274" spans="4:4">
+    <row r="4274" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4274" s="9"/>
     </row>
-    <row r="4275" spans="4:4">
+    <row r="4275" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4275" s="9"/>
     </row>
-    <row r="4276" spans="4:4">
+    <row r="4276" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4276" s="9"/>
     </row>
-    <row r="4277" spans="4:4">
+    <row r="4277" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4277" s="9"/>
     </row>
-    <row r="4278" spans="4:4">
+    <row r="4278" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4278" s="9"/>
     </row>
-    <row r="4279" spans="4:4">
+    <row r="4279" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4279" s="9"/>
     </row>
-    <row r="4280" spans="4:4">
+    <row r="4280" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4280" s="9"/>
     </row>
-    <row r="4281" spans="4:4">
+    <row r="4281" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4281" s="9"/>
     </row>
-    <row r="4282" spans="4:4">
+    <row r="4282" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D4282" s="9"/>
     </row>
   </sheetData>

</xml_diff>